<commit_message>
base of a message handler
</commit_message>
<xml_diff>
--- a/Database/Data/database.xlsx
+++ b/Database/Data/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\PycharmProjects\PirieBot\Database\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B32CC5A-7F38-48C2-A58A-5B9977199883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AA11A6-2B6A-40BE-BEEE-83700D020BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grupos" sheetId="1" r:id="rId1"/>
@@ -197,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="271">
   <si>
     <t>presencial</t>
   </si>
@@ -766,174 +766,6 @@
     <t>fundamentos de la amplificacion de sonido</t>
   </si>
   <si>
-    <t>cardio dance</t>
-  </si>
-  <si>
-    <t>hatha yoga</t>
-  </si>
-  <si>
-    <t>yoga principiantes</t>
-  </si>
-  <si>
-    <t>nutricion inteligente</t>
-  </si>
-  <si>
-    <t>quilting basico</t>
-  </si>
-  <si>
-    <t>pintura oleo</t>
-  </si>
-  <si>
-    <t>pintura acuarela</t>
-  </si>
-  <si>
-    <t>ilustracion mitologica</t>
-  </si>
-  <si>
-    <t>figura humana</t>
-  </si>
-  <si>
-    <t>dibujo artistico 1</t>
-  </si>
-  <si>
-    <t>lettering</t>
-  </si>
-  <si>
-    <t>dibujo manga</t>
-  </si>
-  <si>
-    <t>fotografia digital</t>
-  </si>
-  <si>
-    <t>dibujo manga infantil</t>
-  </si>
-  <si>
-    <t>taller de dibujos animados</t>
-  </si>
-  <si>
-    <t>pintura acrilico</t>
-  </si>
-  <si>
-    <t>dibujo artistico para adultos</t>
-  </si>
-  <si>
-    <t>dibujo artistico infantil</t>
-  </si>
-  <si>
-    <t>taller de dibujo basico infantil</t>
-  </si>
-  <si>
-    <t>creciendo con el arte 2</t>
-  </si>
-  <si>
-    <t>creciendo con el arte 1</t>
-  </si>
-  <si>
-    <t>violin</t>
-  </si>
-  <si>
-    <t>canto popular mixto</t>
-  </si>
-  <si>
-    <t>canto popular 2</t>
-  </si>
-  <si>
-    <t>canto popular 1</t>
-  </si>
-  <si>
-    <t>guitarra clasica (mixto)</t>
-  </si>
-  <si>
-    <t>guitarra popular 3</t>
-  </si>
-  <si>
-    <t>guitarra popular 2</t>
-  </si>
-  <si>
-    <t>guitarra popular 1</t>
-  </si>
-  <si>
-    <t>guitarra popular infantil 3</t>
-  </si>
-  <si>
-    <t>guitarra popular infantil 1</t>
-  </si>
-  <si>
-    <t>ukelele 3</t>
-  </si>
-  <si>
-    <t>ukelele 1</t>
-  </si>
-  <si>
-    <t>ukelele infantil 1</t>
-  </si>
-  <si>
-    <t>organeta popular 1</t>
-  </si>
-  <si>
-    <t>organeta popular infantil 1</t>
-  </si>
-  <si>
-    <t>tribal (mixto)</t>
-  </si>
-  <si>
-    <t>belly dance 3</t>
-  </si>
-  <si>
-    <t>belly dance 2</t>
-  </si>
-  <si>
-    <t>belly dance 1</t>
-  </si>
-  <si>
-    <t>bailes coreograficos</t>
-  </si>
-  <si>
-    <t>compania andanza</t>
-  </si>
-  <si>
-    <t>danza contemporanea</t>
-  </si>
-  <si>
-    <t>ballet y danza juvenil</t>
-  </si>
-  <si>
-    <t>ballet y danza 3</t>
-  </si>
-  <si>
-    <t>ballet y danza 2</t>
-  </si>
-  <si>
-    <t>ballet y danza 1</t>
-  </si>
-  <si>
-    <t>ballet juvenil</t>
-  </si>
-  <si>
-    <t>ballet puntas</t>
-  </si>
-  <si>
-    <t>ballet escolar b</t>
-  </si>
-  <si>
-    <t>ballet escolar a</t>
-  </si>
-  <si>
-    <t>ballet preescolar</t>
-  </si>
-  <si>
-    <t>teatro 3</t>
-  </si>
-  <si>
-    <t>teatro 1</t>
-  </si>
-  <si>
-    <t>teatro infantil 2</t>
-  </si>
-  <si>
-    <t>teatro infantil 1</t>
-  </si>
-  <si>
     <t>Gloriana Quirós</t>
   </si>
   <si>
@@ -1007,16 +839,194 @@
   </si>
   <si>
     <t>Arte y Salud</t>
+  </si>
+  <si>
+    <t>Ballet Escolar B</t>
+  </si>
+  <si>
+    <t>Ballet Pre-Puntas</t>
+  </si>
+  <si>
+    <t>Ballet Puntas</t>
+  </si>
+  <si>
+    <t>Ballet Juvenil</t>
+  </si>
+  <si>
+    <t>Ballet Y Danza 1</t>
+  </si>
+  <si>
+    <t>Ballet Y Danza 2</t>
+  </si>
+  <si>
+    <t>Ballet Y Danza 3</t>
+  </si>
+  <si>
+    <t>Ballet Y Danza Juvenil</t>
+  </si>
+  <si>
+    <t>Danza Contemporanea</t>
+  </si>
+  <si>
+    <t>Compania Andanza</t>
+  </si>
+  <si>
+    <t>Bailes Coreograficos</t>
+  </si>
+  <si>
+    <t>Belly Dance 1</t>
+  </si>
+  <si>
+    <t>Belly Dance 2</t>
+  </si>
+  <si>
+    <t>Belly Dance 3</t>
+  </si>
+  <si>
+    <t>Tribal (Mixto)</t>
+  </si>
+  <si>
+    <t>Organeta Popular Infantil 1</t>
+  </si>
+  <si>
+    <t>Organeta Popular 1</t>
+  </si>
+  <si>
+    <t>Ukelele Infantil 1</t>
+  </si>
+  <si>
+    <t>Ukelele 1</t>
+  </si>
+  <si>
+    <t>Ukelele 3</t>
+  </si>
+  <si>
+    <t>Guitarra Popular Infantil 1</t>
+  </si>
+  <si>
+    <t>Guitarra Popular Infantil 3</t>
+  </si>
+  <si>
+    <t>Guitarra Popular 1</t>
+  </si>
+  <si>
+    <t>Guitarra Popular 2</t>
+  </si>
+  <si>
+    <t>Guitarra Popular 3</t>
+  </si>
+  <si>
+    <t>Guitarra Clasica (Mixto)</t>
+  </si>
+  <si>
+    <t>Canto Popular 1</t>
+  </si>
+  <si>
+    <t>Canto Popular 2</t>
+  </si>
+  <si>
+    <t>Canto Popular Mixto</t>
+  </si>
+  <si>
+    <t>Violin</t>
+  </si>
+  <si>
+    <t>Creciendo Con El Arte 1</t>
+  </si>
+  <si>
+    <t>Creciendo Con El Arte 2</t>
+  </si>
+  <si>
+    <t>Taller De Dibujo Basico Infantil</t>
+  </si>
+  <si>
+    <t>Dibujo Artistico Infantil</t>
+  </si>
+  <si>
+    <t>Dibujo Artistico Para Adultos</t>
+  </si>
+  <si>
+    <t>Pintura Acrilico</t>
+  </si>
+  <si>
+    <t>Taller De Dibujos Animados</t>
+  </si>
+  <si>
+    <t>Dibujo Manga Infantil</t>
+  </si>
+  <si>
+    <t>Pintura Oleo</t>
+  </si>
+  <si>
+    <t>Fotografia Digital</t>
+  </si>
+  <si>
+    <t>Dibujo Manga</t>
+  </si>
+  <si>
+    <t>Lettering</t>
+  </si>
+  <si>
+    <t>Dibujo Artistico 1</t>
+  </si>
+  <si>
+    <t>Figura Humana</t>
+  </si>
+  <si>
+    <t>Ilustracion Mitologica</t>
+  </si>
+  <si>
+    <t>Pintura Acuarela</t>
+  </si>
+  <si>
+    <t>Quilting Basico</t>
+  </si>
+  <si>
+    <t>Nutricion Inteligente</t>
+  </si>
+  <si>
+    <t>Yoga Principiantes</t>
+  </si>
+  <si>
+    <t>Hatha Yoga</t>
+  </si>
+  <si>
+    <t>Cardio Dance</t>
+  </si>
+  <si>
+    <t>Fundamentos De La Amplificacion De Sonido</t>
+  </si>
+  <si>
+    <t>Lesco 1</t>
+  </si>
+  <si>
+    <t>Lesco 2</t>
+  </si>
+  <si>
+    <t>Lesco 3</t>
+  </si>
+  <si>
+    <t>Lesco 4</t>
+  </si>
+  <si>
+    <t>Lesco 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1042,10 +1052,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1458,7 +1471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -4974,8 +4987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2ADEB89-6016-4961-855F-B6B0FA6DB09E}">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4993,8 +5006,8 @@
       <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>244</v>
+      <c r="C1" s="2" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5004,8 +5017,8 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>243</v>
+      <c r="C2" s="2" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5015,8 +5028,8 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>242</v>
+      <c r="C3" s="2" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5026,8 +5039,8 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>241</v>
+      <c r="C4" s="2" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -5037,8 +5050,8 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>240</v>
+      <c r="C5" s="2" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5048,8 +5061,8 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>239</v>
+      <c r="C6" s="2" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5059,8 +5072,8 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>238</v>
+      <c r="C7" s="2" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5070,8 +5083,8 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
-        <v>24</v>
+      <c r="C8" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5081,8 +5094,8 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
-        <v>237</v>
+      <c r="C9" s="2" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5092,8 +5105,8 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
-        <v>236</v>
+      <c r="C10" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5103,8 +5116,8 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
-        <v>235</v>
+      <c r="C11" s="2" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5114,8 +5127,8 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" t="s">
-        <v>234</v>
+      <c r="C12" s="2" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -5125,8 +5138,8 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
-        <v>233</v>
+      <c r="C13" s="2" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5136,8 +5149,8 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
-        <v>232</v>
+      <c r="C14" s="2" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -5147,8 +5160,8 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
-        <v>231</v>
+      <c r="C15" s="2" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5158,8 +5171,8 @@
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
-        <v>230</v>
+      <c r="C16" s="2" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5169,8 +5182,8 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
-        <v>229</v>
+      <c r="C17" s="2" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -5180,7 +5193,7 @@
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>228</v>
       </c>
     </row>
@@ -5191,8 +5204,8 @@
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
-        <v>227</v>
+      <c r="C19" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -5202,8 +5215,8 @@
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" t="s">
-        <v>226</v>
+      <c r="C20" s="2" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -5213,8 +5226,8 @@
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" t="s">
-        <v>228</v>
+      <c r="C21" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -5224,8 +5237,8 @@
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" t="s">
-        <v>227</v>
+      <c r="C22" s="2" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -5235,8 +5248,8 @@
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" t="s">
-        <v>226</v>
+      <c r="C23" s="2" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -5246,8 +5259,8 @@
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
-        <v>225</v>
+      <c r="C24" s="2" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -5257,8 +5270,8 @@
       <c r="B25">
         <v>2</v>
       </c>
-      <c r="C25" t="s">
-        <v>224</v>
+      <c r="C25" s="2" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -5268,8 +5281,8 @@
       <c r="B26">
         <v>2</v>
       </c>
-      <c r="C26" t="s">
-        <v>223</v>
+      <c r="C26" s="2" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -5279,8 +5292,8 @@
       <c r="B27">
         <v>2</v>
       </c>
-      <c r="C27" t="s">
-        <v>222</v>
+      <c r="C27" s="2" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -5290,8 +5303,8 @@
       <c r="B28">
         <v>2</v>
       </c>
-      <c r="C28" t="s">
-        <v>221</v>
+      <c r="C28" s="2" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -5301,8 +5314,8 @@
       <c r="B29">
         <v>2</v>
       </c>
-      <c r="C29" t="s">
-        <v>220</v>
+      <c r="C29" s="2" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -5312,8 +5325,8 @@
       <c r="B30">
         <v>2</v>
       </c>
-      <c r="C30" t="s">
-        <v>219</v>
+      <c r="C30" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -5323,8 +5336,8 @@
       <c r="B31">
         <v>2</v>
       </c>
-      <c r="C31" t="s">
-        <v>218</v>
+      <c r="C31" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -5334,8 +5347,8 @@
       <c r="B32">
         <v>2</v>
       </c>
-      <c r="C32" t="s">
-        <v>217</v>
+      <c r="C32" s="2" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -5345,8 +5358,8 @@
       <c r="B33">
         <v>2</v>
       </c>
-      <c r="C33" t="s">
-        <v>216</v>
+      <c r="C33" s="2" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5356,8 +5369,8 @@
       <c r="B34">
         <v>2</v>
       </c>
-      <c r="C34" t="s">
-        <v>215</v>
+      <c r="C34" s="2" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -5367,8 +5380,8 @@
       <c r="B35">
         <v>2</v>
       </c>
-      <c r="C35" t="s">
-        <v>214</v>
+      <c r="C35" s="2" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5378,8 +5391,8 @@
       <c r="B36">
         <v>2</v>
       </c>
-      <c r="C36" t="s">
-        <v>213</v>
+      <c r="C36" s="2" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -5389,8 +5402,8 @@
       <c r="B37">
         <v>2</v>
       </c>
-      <c r="C37" t="s">
-        <v>212</v>
+      <c r="C37" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -5400,8 +5413,8 @@
       <c r="B38">
         <v>2</v>
       </c>
-      <c r="C38" t="s">
-        <v>211</v>
+      <c r="C38" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5411,8 +5424,8 @@
       <c r="B39">
         <v>2</v>
       </c>
-      <c r="C39" t="s">
-        <v>210</v>
+      <c r="C39" s="2" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -5422,8 +5435,8 @@
       <c r="B40">
         <v>3</v>
       </c>
-      <c r="C40" t="s">
-        <v>209</v>
+      <c r="C40" s="2" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -5433,8 +5446,8 @@
       <c r="B41">
         <v>3</v>
       </c>
-      <c r="C41" t="s">
-        <v>208</v>
+      <c r="C41" s="2" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -5444,8 +5457,8 @@
       <c r="B42">
         <v>3</v>
       </c>
-      <c r="C42" t="s">
-        <v>207</v>
+      <c r="C42" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -5455,8 +5468,8 @@
       <c r="B43">
         <v>3</v>
       </c>
-      <c r="C43" t="s">
-        <v>206</v>
+      <c r="C43" s="2" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -5466,8 +5479,8 @@
       <c r="B44">
         <v>3</v>
       </c>
-      <c r="C44" t="s">
-        <v>205</v>
+      <c r="C44" s="2" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -5477,8 +5490,8 @@
       <c r="B45">
         <v>3</v>
       </c>
-      <c r="C45" t="s">
-        <v>204</v>
+      <c r="C45" s="2" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -5488,8 +5501,8 @@
       <c r="B46">
         <v>3</v>
       </c>
-      <c r="C46" t="s">
-        <v>203</v>
+      <c r="C46" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -5499,8 +5512,8 @@
       <c r="B47">
         <v>3</v>
       </c>
-      <c r="C47" t="s">
-        <v>202</v>
+      <c r="C47" s="2" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5510,8 +5523,8 @@
       <c r="B48">
         <v>3</v>
       </c>
-      <c r="C48" t="s">
-        <v>194</v>
+      <c r="C48" s="2" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -5521,8 +5534,8 @@
       <c r="B49">
         <v>3</v>
       </c>
-      <c r="C49" t="s">
-        <v>201</v>
+      <c r="C49" s="2" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -5532,8 +5545,8 @@
       <c r="B50">
         <v>3</v>
       </c>
-      <c r="C50" t="s">
-        <v>200</v>
+      <c r="C50" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5543,8 +5556,8 @@
       <c r="B51">
         <v>3</v>
       </c>
-      <c r="C51" t="s">
-        <v>199</v>
+      <c r="C51" s="2" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -5554,8 +5567,8 @@
       <c r="B52">
         <v>3</v>
       </c>
-      <c r="C52" t="s">
-        <v>198</v>
+      <c r="C52" s="2" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5565,8 +5578,8 @@
       <c r="B53">
         <v>3</v>
       </c>
-      <c r="C53" t="s">
-        <v>197</v>
+      <c r="C53" s="2" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5576,8 +5589,8 @@
       <c r="B54">
         <v>3</v>
       </c>
-      <c r="C54" t="s">
-        <v>196</v>
+      <c r="C54" s="2" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5587,8 +5600,8 @@
       <c r="B55">
         <v>3</v>
       </c>
-      <c r="C55" t="s">
-        <v>195</v>
+      <c r="C55" s="2" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -5598,8 +5611,8 @@
       <c r="B56">
         <v>3</v>
       </c>
-      <c r="C56" t="s">
-        <v>194</v>
+      <c r="C56" s="2" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -5609,8 +5622,8 @@
       <c r="B57">
         <v>4</v>
       </c>
-      <c r="C57" t="s">
-        <v>193</v>
+      <c r="C57" s="2" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -5620,8 +5633,8 @@
       <c r="B58">
         <v>5</v>
       </c>
-      <c r="C58" t="s">
-        <v>192</v>
+      <c r="C58" s="2" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -5631,8 +5644,8 @@
       <c r="B59">
         <v>5</v>
       </c>
-      <c r="C59" t="s">
-        <v>191</v>
+      <c r="C59" s="2" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -5642,8 +5655,8 @@
       <c r="B60">
         <v>5</v>
       </c>
-      <c r="C60" t="s">
-        <v>190</v>
+      <c r="C60" s="2" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -5653,8 +5666,8 @@
       <c r="B61">
         <v>5</v>
       </c>
-      <c r="C61" t="s">
-        <v>189</v>
+      <c r="C61" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -5725,7 +5738,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5749,7 +5763,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>245</v>
+        <v>189</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -5758,7 +5772,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>246</v>
+        <v>190</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -5767,7 +5781,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>247</v>
+        <v>191</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -5776,7 +5790,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -5785,7 +5799,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>249</v>
+        <v>193</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -5794,7 +5808,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>250</v>
+        <v>194</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -5803,7 +5817,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>251</v>
+        <v>195</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -5812,7 +5826,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>252</v>
+        <v>196</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -5821,7 +5835,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
+        <v>197</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -5830,7 +5844,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>254</v>
+        <v>198</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -5839,7 +5853,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>255</v>
+        <v>199</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -5848,7 +5862,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>256</v>
+        <v>200</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -5857,7 +5871,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>263</v>
+        <v>207</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -5866,7 +5880,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>257</v>
+        <v>201</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -5875,7 +5889,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>258</v>
+        <v>202</v>
       </c>
       <c r="C15" s="1"/>
     </row>
@@ -5884,7 +5898,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>259</v>
+        <v>203</v>
       </c>
       <c r="C16" s="1"/>
     </row>
@@ -5893,7 +5907,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>260</v>
+        <v>204</v>
       </c>
       <c r="C17" s="1"/>
     </row>
@@ -5902,7 +5916,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>261</v>
+        <v>205</v>
       </c>
       <c r="C18" s="1"/>
     </row>
@@ -5911,7 +5925,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>262</v>
+        <v>206</v>
       </c>
       <c r="C19" s="1"/>
     </row>
@@ -5920,7 +5934,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>253</v>
+        <v>197</v>
       </c>
       <c r="C20" s="1"/>
     </row>
@@ -5929,7 +5943,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="C21" s="1"/>
     </row>
@@ -5955,32 +5969,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>264</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>268</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>269</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new comments on database
</commit_message>
<xml_diff>
--- a/Database/Data/database.xlsx
+++ b/Database/Data/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\PycharmProjects\PirieBot\Database\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2746E061-4F0A-4613-AD97-44C8BA098A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162A6E46-04D7-4785-89C6-81441FB2B68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grupos" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,6 @@
     <author>tc={CAF723D9-8235-4372-8427-1B675BCE4B79}</author>
     <author>tc={068B5026-5D55-4C36-A823-582BA669CCFB}</author>
     <author>tc={ADC17C23-7453-472E-B80A-E8861912AE14}</author>
-    <author>tc={C45B0931-04BB-44A3-8A1F-A1DD90B9846C}</author>
     <author>tc={434D33C9-6396-431B-A06B-604CE68627A9}</author>
   </authors>
   <commentList>
@@ -95,15 +94,7 @@
     class</t>
       </text>
     </comment>
-    <comment ref="H1" authorId="7" shapeId="0" xr:uid="{C45B0931-04BB-44A3-8A1F-A1DD90B9846C}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    recomendations</t>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="8" shapeId="0" xr:uid="{434D33C9-6396-431B-A06B-604CE68627A9}">
+    <comment ref="H1" authorId="7" shapeId="0" xr:uid="{434D33C9-6396-431B-A06B-604CE68627A9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -121,6 +112,8 @@
     <author>tc={948D2A91-26FC-4A9E-A133-BFA6225ED9FD}</author>
     <author>tc={665BE74B-730A-4B41-B168-3B8E6ABFE40B}</author>
     <author>tc={B3D325A7-DD65-451D-975F-32B8A78690EE}</author>
+    <author>tc={40FE144C-D2CB-4BCE-B7E5-E087CBF13956}</author>
+    <author>tc={BA83BE48-2326-4572-B975-ED8DFC153836}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{948D2A91-26FC-4A9E-A133-BFA6225ED9FD}">
@@ -147,6 +140,22 @@
     course_name</t>
       </text>
     </comment>
+    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{40FE144C-D2CB-4BCE-B7E5-E087CBF13956}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    recomendations</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{BA83BE48-2326-4572-B975-ED8DFC153836}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    description</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -156,6 +165,7 @@
   <authors>
     <author>tc={B5303C35-FD6F-46CF-A128-046D190393C2}</author>
     <author>tc={3B3177C4-D270-4B53-BA3A-029D244BE86E}</author>
+    <author>tc={DC541F61-3F9E-4EF6-AB65-59B9FBA3E79B}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B5303C35-FD6F-46CF-A128-046D190393C2}">
@@ -172,6 +182,14 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     teacher_name</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{DC541F61-3F9E-4EF6-AB65-59B9FBA3E79B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    bio</t>
       </text>
     </comment>
   </commentList>
@@ -1425,10 +1443,7 @@
   <threadedComment ref="G1" dT="2023-03-05T18:45:52.80" personId="{6DF7EF9A-B3A0-4845-92B8-B81FE36C707F}" id="{ADC17C23-7453-472E-B80A-E8861912AE14}">
     <text>class</text>
   </threadedComment>
-  <threadedComment ref="H1" dT="2023-03-05T21:10:24.40" personId="{6DF7EF9A-B3A0-4845-92B8-B81FE36C707F}" id="{C45B0931-04BB-44A3-8A1F-A1DD90B9846C}">
-    <text>recomendations</text>
-  </threadedComment>
-  <threadedComment ref="I1" dT="2023-03-05T21:11:21.65" personId="{6DF7EF9A-B3A0-4845-92B8-B81FE36C707F}" id="{434D33C9-6396-431B-A06B-604CE68627A9}">
+  <threadedComment ref="H1" dT="2023-03-05T21:11:21.65" personId="{6DF7EF9A-B3A0-4845-92B8-B81FE36C707F}" id="{434D33C9-6396-431B-A06B-604CE68627A9}">
     <text>availibility</text>
   </threadedComment>
 </ThreadedComments>
@@ -1445,6 +1460,12 @@
   <threadedComment ref="C1" dT="2023-03-05T18:43:09.76" personId="{6DF7EF9A-B3A0-4845-92B8-B81FE36C707F}" id="{B3D325A7-DD65-451D-975F-32B8A78690EE}">
     <text>course_name</text>
   </threadedComment>
+  <threadedComment ref="D1" dT="2023-03-24T20:53:08.18" personId="{6DF7EF9A-B3A0-4845-92B8-B81FE36C707F}" id="{40FE144C-D2CB-4BCE-B7E5-E087CBF13956}">
+    <text>recomendations</text>
+  </threadedComment>
+  <threadedComment ref="E1" dT="2023-03-24T20:53:49.73" personId="{6DF7EF9A-B3A0-4845-92B8-B81FE36C707F}" id="{BA83BE48-2326-4572-B975-ED8DFC153836}">
+    <text>description</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1455,6 +1476,9 @@
   </threadedComment>
   <threadedComment ref="B1" dT="2023-03-05T18:42:03.10" personId="{6DF7EF9A-B3A0-4845-92B8-B81FE36C707F}" id="{3B3177C4-D270-4B53-BA3A-029D244BE86E}">
     <text>teacher_name</text>
+  </threadedComment>
+  <threadedComment ref="C1" dT="2023-03-24T20:54:25.78" personId="{6DF7EF9A-B3A0-4845-92B8-B81FE36C707F}" id="{DC541F61-3F9E-4EF6-AB65-59B9FBA3E79B}">
+    <text>bio</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1469,10 +1493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I156"/>
+  <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D157" sqref="D157"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I153" sqref="I153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,7 +1510,7 @@
     <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -1508,8 +1532,11 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -1531,8 +1558,11 @@
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -1552,8 +1582,11 @@
         <v>2</v>
       </c>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1575,8 +1608,11 @@
       <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1598,8 +1634,11 @@
       <c r="G5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1621,8 +1660,11 @@
       <c r="G6" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1644,8 +1686,11 @@
       <c r="G7" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1667,8 +1712,11 @@
       <c r="G8" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1690,8 +1738,11 @@
       <c r="G9" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1713,8 +1764,11 @@
       <c r="G10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1736,8 +1790,11 @@
       <c r="G11" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1759,8 +1816,11 @@
       <c r="G12" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1782,8 +1842,11 @@
       <c r="G13" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1805,8 +1868,11 @@
       <c r="G14" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -1828,8 +1894,11 @@
       <c r="G15" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>11</v>
       </c>
@@ -1851,8 +1920,11 @@
       <c r="G16" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>12</v>
       </c>
@@ -1874,8 +1946,11 @@
       <c r="G17" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>12</v>
       </c>
@@ -1897,8 +1972,11 @@
       <c r="G18" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>13</v>
       </c>
@@ -1920,8 +1998,11 @@
       <c r="G19" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>14</v>
       </c>
@@ -1943,8 +2024,11 @@
       <c r="G20" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>15</v>
       </c>
@@ -1966,8 +2050,11 @@
       <c r="G21" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>16</v>
       </c>
@@ -1989,8 +2076,11 @@
       <c r="G22" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>17</v>
       </c>
@@ -2012,8 +2102,11 @@
       <c r="G23" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>18</v>
       </c>
@@ -2035,8 +2128,11 @@
       <c r="G24" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>18</v>
       </c>
@@ -2058,8 +2154,11 @@
       <c r="G25" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>18</v>
       </c>
@@ -2079,8 +2178,11 @@
         <v>2</v>
       </c>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>18</v>
       </c>
@@ -2102,8 +2204,11 @@
       <c r="G27" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>18</v>
       </c>
@@ -2125,8 +2230,11 @@
       <c r="G28" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>19</v>
       </c>
@@ -2148,8 +2256,11 @@
       <c r="G29" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>19</v>
       </c>
@@ -2171,8 +2282,11 @@
       <c r="G30" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>19</v>
       </c>
@@ -2192,8 +2306,11 @@
         <v>2</v>
       </c>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>20</v>
       </c>
@@ -2215,8 +2332,11 @@
       <c r="G32" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>20</v>
       </c>
@@ -2238,8 +2358,11 @@
       <c r="G33" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>20</v>
       </c>
@@ -2261,8 +2384,11 @@
       <c r="G34" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>24</v>
       </c>
@@ -2284,8 +2410,11 @@
       <c r="G35" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>25</v>
       </c>
@@ -2307,8 +2436,11 @@
       <c r="G36" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>26</v>
       </c>
@@ -2330,8 +2462,11 @@
       <c r="G37" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>26</v>
       </c>
@@ -2353,8 +2488,11 @@
       <c r="G38" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>27</v>
       </c>
@@ -2376,8 +2514,11 @@
       <c r="G39" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>28</v>
       </c>
@@ -2399,8 +2540,11 @@
       <c r="G40" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>29</v>
       </c>
@@ -2422,8 +2566,11 @@
       <c r="G41" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>30</v>
       </c>
@@ -2445,8 +2592,11 @@
       <c r="G42" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>31</v>
       </c>
@@ -2466,8 +2616,11 @@
         <v>2</v>
       </c>
       <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>32</v>
       </c>
@@ -2489,8 +2642,11 @@
       <c r="G44" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>32</v>
       </c>
@@ -2512,8 +2668,11 @@
       <c r="G45" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>33</v>
       </c>
@@ -2535,8 +2694,11 @@
       <c r="G46" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>34</v>
       </c>
@@ -2558,8 +2720,11 @@
       <c r="G47" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>35</v>
       </c>
@@ -2579,8 +2744,11 @@
         <v>12</v>
       </c>
       <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>35</v>
       </c>
@@ -2600,8 +2768,11 @@
         <v>12</v>
       </c>
       <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>35</v>
       </c>
@@ -2621,8 +2792,11 @@
         <v>12</v>
       </c>
       <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>35</v>
       </c>
@@ -2642,8 +2816,11 @@
         <v>12</v>
       </c>
       <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>35</v>
       </c>
@@ -2663,8 +2840,11 @@
         <v>12</v>
       </c>
       <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>35</v>
       </c>
@@ -2684,8 +2864,11 @@
         <v>12</v>
       </c>
       <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>35</v>
       </c>
@@ -2705,8 +2888,11 @@
         <v>12</v>
       </c>
       <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>35</v>
       </c>
@@ -2728,8 +2914,11 @@
       <c r="G55" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>35</v>
       </c>
@@ -2751,8 +2940,11 @@
       <c r="G56" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>35</v>
       </c>
@@ -2774,8 +2966,11 @@
       <c r="G57" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>35</v>
       </c>
@@ -2797,8 +2992,11 @@
       <c r="G58" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>35</v>
       </c>
@@ -2820,8 +3018,11 @@
       <c r="G59" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>35</v>
       </c>
@@ -2843,8 +3044,11 @@
       <c r="G60" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>35</v>
       </c>
@@ -2866,8 +3070,11 @@
       <c r="G61" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>35</v>
       </c>
@@ -2887,8 +3094,11 @@
         <v>12</v>
       </c>
       <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>35</v>
       </c>
@@ -2908,8 +3118,11 @@
         <v>12</v>
       </c>
       <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>35</v>
       </c>
@@ -2929,8 +3142,11 @@
         <v>12</v>
       </c>
       <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>35</v>
       </c>
@@ -2950,8 +3166,11 @@
         <v>12</v>
       </c>
       <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>35</v>
       </c>
@@ -2971,8 +3190,11 @@
         <v>12</v>
       </c>
       <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>35</v>
       </c>
@@ -2992,8 +3214,11 @@
         <v>12</v>
       </c>
       <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>35</v>
       </c>
@@ -3013,8 +3238,11 @@
         <v>12</v>
       </c>
       <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>35</v>
       </c>
@@ -3036,8 +3264,11 @@
       <c r="G69" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>35</v>
       </c>
@@ -3059,8 +3290,11 @@
       <c r="G70" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>35</v>
       </c>
@@ -3082,8 +3316,11 @@
       <c r="G71" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>35</v>
       </c>
@@ -3105,8 +3342,11 @@
       <c r="G72" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>35</v>
       </c>
@@ -3128,8 +3368,11 @@
       <c r="G73" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>35</v>
       </c>
@@ -3151,8 +3394,11 @@
       <c r="G74" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>35</v>
       </c>
@@ -3174,8 +3420,11 @@
       <c r="G75" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>35</v>
       </c>
@@ -3197,8 +3446,11 @@
       <c r="G76" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>35</v>
       </c>
@@ -3220,8 +3472,11 @@
       <c r="G77" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>35</v>
       </c>
@@ -3243,8 +3498,11 @@
       <c r="G78" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>35</v>
       </c>
@@ -3266,8 +3524,11 @@
       <c r="G79" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>35</v>
       </c>
@@ -3289,8 +3550,11 @@
       <c r="G80" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>35</v>
       </c>
@@ -3312,8 +3576,11 @@
       <c r="G81" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>35</v>
       </c>
@@ -3335,8 +3602,11 @@
       <c r="G82" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>36</v>
       </c>
@@ -3358,8 +3628,11 @@
       <c r="G83" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>36</v>
       </c>
@@ -3379,8 +3652,11 @@
         <v>2</v>
       </c>
       <c r="G84" s="1"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>36</v>
       </c>
@@ -3402,8 +3678,11 @@
       <c r="G85" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>36</v>
       </c>
@@ -3425,8 +3704,11 @@
       <c r="G86" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>37</v>
       </c>
@@ -3446,8 +3728,11 @@
         <v>2</v>
       </c>
       <c r="G87" s="1"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>37</v>
       </c>
@@ -3467,8 +3752,11 @@
         <v>2</v>
       </c>
       <c r="G88" s="1"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>38</v>
       </c>
@@ -3490,8 +3778,11 @@
       <c r="G89" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>39</v>
       </c>
@@ -3511,8 +3802,11 @@
         <v>2</v>
       </c>
       <c r="G90" s="1"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>39</v>
       </c>
@@ -3532,8 +3826,11 @@
         <v>2</v>
       </c>
       <c r="G91" s="1"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>39</v>
       </c>
@@ -3553,8 +3850,11 @@
         <v>2</v>
       </c>
       <c r="G92" s="1"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>40</v>
       </c>
@@ -3574,8 +3874,11 @@
         <v>12</v>
       </c>
       <c r="G93" s="1"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>40</v>
       </c>
@@ -3597,8 +3900,11 @@
       <c r="G94" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>40</v>
       </c>
@@ -3620,8 +3926,11 @@
       <c r="G95" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>41</v>
       </c>
@@ -3641,8 +3950,11 @@
         <v>12</v>
       </c>
       <c r="G96" s="1"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>41</v>
       </c>
@@ -3664,8 +3976,11 @@
       <c r="G97" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>42</v>
       </c>
@@ -3685,8 +4000,11 @@
         <v>12</v>
       </c>
       <c r="G98" s="1"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>42</v>
       </c>
@@ -3708,8 +4026,11 @@
       <c r="G99" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>43</v>
       </c>
@@ -3729,8 +4050,11 @@
         <v>12</v>
       </c>
       <c r="G100" s="1"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>43</v>
       </c>
@@ -3752,8 +4076,11 @@
       <c r="G101" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>46</v>
       </c>
@@ -3775,8 +4102,11 @@
       <c r="G102" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>47</v>
       </c>
@@ -3796,8 +4126,11 @@
         <v>2</v>
       </c>
       <c r="G103" s="1"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>47</v>
       </c>
@@ -3817,8 +4150,11 @@
         <v>2</v>
       </c>
       <c r="G104" s="1"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>47</v>
       </c>
@@ -3840,8 +4176,11 @@
       <c r="G105" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>47</v>
       </c>
@@ -3863,8 +4202,11 @@
       <c r="G106" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>49</v>
       </c>
@@ -3886,8 +4228,11 @@
       <c r="G107" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>50</v>
       </c>
@@ -3909,8 +4254,11 @@
       <c r="G108" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>51</v>
       </c>
@@ -3932,8 +4280,11 @@
       <c r="G109" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44</v>
       </c>
@@ -3955,8 +4306,11 @@
       <c r="G110" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>52</v>
       </c>
@@ -3978,8 +4332,11 @@
       <c r="G111" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>52</v>
       </c>
@@ -4001,8 +4358,11 @@
       <c r="G112" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>53</v>
       </c>
@@ -4024,8 +4384,11 @@
       <c r="G113" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>54</v>
       </c>
@@ -4047,8 +4410,11 @@
       <c r="G114" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>55</v>
       </c>
@@ -4070,8 +4436,11 @@
       <c r="G115" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>55</v>
       </c>
@@ -4091,8 +4460,11 @@
         <v>12</v>
       </c>
       <c r="G116" s="1"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>45</v>
       </c>
@@ -4114,8 +4486,11 @@
       <c r="G117" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>45</v>
       </c>
@@ -4135,8 +4510,11 @@
         <v>12</v>
       </c>
       <c r="G118" s="1"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>48</v>
       </c>
@@ -4158,8 +4536,11 @@
       <c r="G119" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>48</v>
       </c>
@@ -4179,8 +4560,11 @@
         <v>12</v>
       </c>
       <c r="G120" s="1"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>48</v>
       </c>
@@ -4202,8 +4586,11 @@
       <c r="G121" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>48</v>
       </c>
@@ -4225,8 +4612,11 @@
       <c r="G122" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>48</v>
       </c>
@@ -4248,8 +4638,11 @@
       <c r="G123" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>57</v>
       </c>
@@ -4269,8 +4662,11 @@
         <v>2</v>
       </c>
       <c r="G124" s="1"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>57</v>
       </c>
@@ -4290,8 +4686,11 @@
         <v>2</v>
       </c>
       <c r="G125" s="1"/>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>57</v>
       </c>
@@ -4311,8 +4710,11 @@
         <v>2</v>
       </c>
       <c r="G126" s="1"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>57</v>
       </c>
@@ -4334,8 +4736,11 @@
       <c r="G127" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>57</v>
       </c>
@@ -4357,8 +4762,11 @@
       <c r="G128" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>57</v>
       </c>
@@ -4380,8 +4788,11 @@
       <c r="G129" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>57</v>
       </c>
@@ -4403,8 +4814,11 @@
       <c r="G130" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>58</v>
       </c>
@@ -4424,8 +4838,11 @@
         <v>148</v>
       </c>
       <c r="G131" s="1"/>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>59</v>
       </c>
@@ -4447,8 +4864,11 @@
       <c r="G132" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>59</v>
       </c>
@@ -4470,8 +4890,11 @@
       <c r="G133" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>60</v>
       </c>
@@ -4493,8 +4916,11 @@
       <c r="G134" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>60</v>
       </c>
@@ -4516,8 +4942,11 @@
       <c r="G135" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>60</v>
       </c>
@@ -4539,8 +4968,11 @@
       <c r="G136" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>61</v>
       </c>
@@ -4560,8 +4992,11 @@
         <v>2</v>
       </c>
       <c r="G137" s="1"/>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>61</v>
       </c>
@@ -4581,8 +5016,11 @@
         <v>2</v>
       </c>
       <c r="G138" s="1"/>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>61</v>
       </c>
@@ -4602,8 +5040,11 @@
         <v>2</v>
       </c>
       <c r="G139" s="1"/>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>62</v>
       </c>
@@ -4625,8 +5066,11 @@
       <c r="G140" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>62</v>
       </c>
@@ -4648,8 +5092,11 @@
       <c r="G141" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>63</v>
       </c>
@@ -4669,8 +5116,11 @@
         <v>148</v>
       </c>
       <c r="G142" s="1"/>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>63</v>
       </c>
@@ -4692,8 +5142,11 @@
       <c r="G143" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>63</v>
       </c>
@@ -4715,8 +5168,11 @@
       <c r="G144" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>63</v>
       </c>
@@ -4736,8 +5192,11 @@
         <v>148</v>
       </c>
       <c r="G145" s="1"/>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>63</v>
       </c>
@@ -4757,8 +5216,11 @@
         <v>148</v>
       </c>
       <c r="G146" s="1"/>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>63</v>
       </c>
@@ -4778,8 +5240,11 @@
         <v>148</v>
       </c>
       <c r="G147" s="1"/>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>63</v>
       </c>
@@ -4799,8 +5264,11 @@
         <v>148</v>
       </c>
       <c r="G148" s="1"/>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>63</v>
       </c>
@@ -4820,8 +5288,11 @@
         <v>148</v>
       </c>
       <c r="G149" s="1"/>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>63</v>
       </c>
@@ -4843,8 +5314,11 @@
       <c r="G150" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>64</v>
       </c>
@@ -4866,8 +5340,11 @@
       <c r="G151" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>65</v>
       </c>
@@ -4889,8 +5366,11 @@
       <c r="G152" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>65</v>
       </c>
@@ -4910,8 +5390,11 @@
         <v>148</v>
       </c>
       <c r="G153" s="1"/>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>66</v>
       </c>
@@ -4931,8 +5414,11 @@
         <v>148</v>
       </c>
       <c r="G154" s="1"/>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>66</v>
       </c>
@@ -4952,8 +5438,11 @@
         <v>148</v>
       </c>
       <c r="G155" s="1"/>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>67</v>
       </c>
@@ -4973,6 +5462,9 @@
         <v>148</v>
       </c>
       <c r="G156" s="1"/>
+      <c r="H156">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4985,10 +5477,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2ADEB89-6016-4961-855F-B6B0FA6DB09E}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4999,7 +5491,7 @@
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -5010,7 +5502,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5021,7 +5513,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5032,7 +5524,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5043,7 +5535,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -5054,7 +5546,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -5065,7 +5557,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -5076,7 +5568,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -5087,7 +5579,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -5098,7 +5590,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -5109,7 +5601,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -5120,7 +5612,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -5131,7 +5623,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -5142,7 +5634,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -5153,7 +5645,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -5164,7 +5656,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -5747,8 +6239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B558BCCB-B295-4555-AF6A-EC02D1057D3C}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5989,12 +6481,12 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nuevos cursos de lesco y mensaje adaptado a dar más información
</commit_message>
<xml_diff>
--- a/Database/Data/database.xlsx
+++ b/Database/Data/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\PycharmProjects\PirieBot\Database\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162A6E46-04D7-4785-89C6-81441FB2B68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A64B13A-35B1-4E2A-AEDA-6EDD07233520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grupos" sheetId="1" r:id="rId1"/>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="277">
   <si>
     <t>S: 10:30 am - 11:30 am</t>
   </si>
@@ -1025,13 +1025,34 @@
   </si>
   <si>
     <t>Nutrición Inteligente</t>
+  </si>
+  <si>
+    <t>Lesco 5</t>
+  </si>
+  <si>
+    <t>J: 9:00 am - 12:00 md</t>
+  </si>
+  <si>
+    <t>V: 6:00 pm - 9:00 pm</t>
+  </si>
+  <si>
+    <t>V: 9:00 am - 12:00 md</t>
+  </si>
+  <si>
+    <t>V: 2:00 pm -5:00 pm</t>
+  </si>
+  <si>
+    <t>El curso de lengua de señas costarricense tiene el propósito de proveer a los estudiantes la adquisición de elementos básicos de la lengua y proveer las competencias básicas en la lengua de señas costarricenses.</t>
+  </si>
+  <si>
+    <t>Este curso es reconocido por el Servicio Civil por lo que es importante que no faltes a las clases o justifiques y repongas las lecciones a las que te ausentes.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1042,6 +1063,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1073,10 +1100,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1493,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H156"/>
+  <dimension ref="A1:H170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I153" sqref="I153"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I156" sqref="I156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,7 +1541,7 @@
       <c r="A1" s="1">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C1" s="1">
@@ -1540,7 +1567,7 @@
       <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C2" s="1">
@@ -1566,7 +1593,7 @@
       <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C3" s="1">
@@ -1590,7 +1617,7 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C4" s="1">
@@ -1616,7 +1643,7 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C5" s="1">
@@ -1642,7 +1669,7 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C6" s="1">
@@ -1668,7 +1695,7 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C7" s="1">
@@ -1694,7 +1721,7 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C8" s="1">
@@ -1720,7 +1747,7 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C9" s="1">
@@ -1746,7 +1773,7 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C10" s="1">
@@ -1772,7 +1799,7 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C11" s="1">
@@ -1798,7 +1825,7 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C12" s="1">
@@ -1824,7 +1851,7 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C13" s="1">
@@ -1850,7 +1877,7 @@
       <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C14" s="1">
@@ -1876,7 +1903,7 @@
       <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C15" s="1">
@@ -1902,7 +1929,7 @@
       <c r="A16" s="1">
         <v>11</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C16" s="1">
@@ -1928,7 +1955,7 @@
       <c r="A17" s="1">
         <v>12</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C17" s="1">
@@ -1954,7 +1981,7 @@
       <c r="A18" s="1">
         <v>12</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C18" s="1">
@@ -1980,7 +2007,7 @@
       <c r="A19" s="1">
         <v>13</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C19" s="1">
@@ -2006,7 +2033,7 @@
       <c r="A20" s="1">
         <v>14</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C20" s="1">
@@ -2032,7 +2059,7 @@
       <c r="A21" s="1">
         <v>15</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C21" s="1">
@@ -2058,7 +2085,7 @@
       <c r="A22" s="1">
         <v>16</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C22" s="1">
@@ -2084,7 +2111,7 @@
       <c r="A23" s="1">
         <v>17</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C23" s="1">
@@ -2110,7 +2137,7 @@
       <c r="A24" s="1">
         <v>18</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C24" s="1">
@@ -2136,7 +2163,7 @@
       <c r="A25" s="1">
         <v>18</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C25" s="1">
@@ -2162,7 +2189,7 @@
       <c r="A26" s="1">
         <v>18</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C26" s="1">
@@ -2186,7 +2213,7 @@
       <c r="A27" s="1">
         <v>18</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C27" s="1">
@@ -2212,7 +2239,7 @@
       <c r="A28" s="1">
         <v>18</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C28" s="1">
@@ -2238,7 +2265,7 @@
       <c r="A29" s="1">
         <v>19</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C29" s="1">
@@ -2264,7 +2291,7 @@
       <c r="A30" s="1">
         <v>19</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C30" s="1">
@@ -2290,7 +2317,7 @@
       <c r="A31" s="1">
         <v>19</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C31" s="1">
@@ -2314,7 +2341,7 @@
       <c r="A32" s="1">
         <v>20</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C32" s="1">
@@ -2340,7 +2367,7 @@
       <c r="A33" s="1">
         <v>20</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C33" s="1">
@@ -2366,7 +2393,7 @@
       <c r="A34" s="1">
         <v>20</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C34" s="1">
@@ -2392,7 +2419,7 @@
       <c r="A35" s="1">
         <v>24</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C35" s="1">
@@ -2418,7 +2445,7 @@
       <c r="A36" s="1">
         <v>25</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C36" s="1">
@@ -2444,7 +2471,7 @@
       <c r="A37" s="1">
         <v>26</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C37" s="1">
@@ -2470,7 +2497,7 @@
       <c r="A38" s="1">
         <v>26</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C38" s="1">
@@ -2496,7 +2523,7 @@
       <c r="A39" s="1">
         <v>27</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C39" s="1">
@@ -2522,7 +2549,7 @@
       <c r="A40" s="1">
         <v>28</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C40" s="1">
@@ -2548,7 +2575,7 @@
       <c r="A41" s="1">
         <v>29</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C41" s="1">
@@ -2574,7 +2601,7 @@
       <c r="A42" s="1">
         <v>30</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C42" s="1">
@@ -2600,7 +2627,7 @@
       <c r="A43" s="1">
         <v>31</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C43" s="1">
@@ -2624,7 +2651,7 @@
       <c r="A44" s="1">
         <v>32</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C44" s="1">
@@ -2650,7 +2677,7 @@
       <c r="A45" s="1">
         <v>32</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C45" s="1">
@@ -2676,7 +2703,7 @@
       <c r="A46" s="1">
         <v>33</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C46" s="1">
@@ -2702,7 +2729,7 @@
       <c r="A47" s="1">
         <v>34</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C47" s="1">
@@ -2728,7 +2755,7 @@
       <c r="A48" s="1">
         <v>35</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C48" s="1">
@@ -2752,7 +2779,7 @@
       <c r="A49" s="1">
         <v>35</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C49" s="1">
@@ -2776,7 +2803,7 @@
       <c r="A50" s="1">
         <v>35</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C50" s="1">
@@ -2800,7 +2827,7 @@
       <c r="A51" s="1">
         <v>35</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C51" s="1">
@@ -2824,7 +2851,7 @@
       <c r="A52" s="1">
         <v>35</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C52" s="1">
@@ -2848,7 +2875,7 @@
       <c r="A53" s="1">
         <v>35</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C53" s="1">
@@ -2872,7 +2899,7 @@
       <c r="A54" s="1">
         <v>35</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C54" s="1">
@@ -2896,7 +2923,7 @@
       <c r="A55" s="1">
         <v>35</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C55" s="1">
@@ -2922,7 +2949,7 @@
       <c r="A56" s="1">
         <v>35</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C56" s="1">
@@ -2948,7 +2975,7 @@
       <c r="A57" s="1">
         <v>35</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C57" s="1">
@@ -2974,7 +3001,7 @@
       <c r="A58" s="1">
         <v>35</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C58" s="1">
@@ -3000,7 +3027,7 @@
       <c r="A59" s="1">
         <v>35</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C59" s="1">
@@ -3026,7 +3053,7 @@
       <c r="A60" s="1">
         <v>35</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C60" s="1">
@@ -3052,7 +3079,7 @@
       <c r="A61" s="1">
         <v>35</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C61" s="1">
@@ -3078,7 +3105,7 @@
       <c r="A62" s="1">
         <v>35</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C62" s="1">
@@ -3102,7 +3129,7 @@
       <c r="A63" s="1">
         <v>35</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C63" s="1">
@@ -3126,7 +3153,7 @@
       <c r="A64" s="1">
         <v>35</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C64" s="1">
@@ -3150,7 +3177,7 @@
       <c r="A65" s="1">
         <v>35</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C65" s="1">
@@ -3174,7 +3201,7 @@
       <c r="A66" s="1">
         <v>35</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C66" s="1">
@@ -3198,7 +3225,7 @@
       <c r="A67" s="1">
         <v>35</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C67" s="1">
@@ -3222,7 +3249,7 @@
       <c r="A68" s="1">
         <v>35</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C68" s="1">
@@ -3246,7 +3273,7 @@
       <c r="A69" s="1">
         <v>35</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C69" s="1">
@@ -3272,7 +3299,7 @@
       <c r="A70" s="1">
         <v>35</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C70" s="1">
@@ -3298,7 +3325,7 @@
       <c r="A71" s="1">
         <v>35</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C71" s="1">
@@ -3324,7 +3351,7 @@
       <c r="A72" s="1">
         <v>35</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C72" s="1">
@@ -3350,7 +3377,7 @@
       <c r="A73" s="1">
         <v>35</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C73" s="1">
@@ -3376,7 +3403,7 @@
       <c r="A74" s="1">
         <v>35</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C74" s="1">
@@ -3402,7 +3429,7 @@
       <c r="A75" s="1">
         <v>35</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C75" s="1">
@@ -3428,7 +3455,7 @@
       <c r="A76" s="1">
         <v>35</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C76" s="1">
@@ -3454,7 +3481,7 @@
       <c r="A77" s="1">
         <v>35</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C77" s="1">
@@ -3480,7 +3507,7 @@
       <c r="A78" s="1">
         <v>35</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C78" s="1">
@@ -3506,7 +3533,7 @@
       <c r="A79" s="1">
         <v>35</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C79" s="1">
@@ -3532,7 +3559,7 @@
       <c r="A80" s="1">
         <v>35</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C80" s="1">
@@ -3558,7 +3585,7 @@
       <c r="A81" s="1">
         <v>35</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C81" s="1">
@@ -3584,7 +3611,7 @@
       <c r="A82" s="1">
         <v>35</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C82" s="1">
@@ -3610,7 +3637,7 @@
       <c r="A83" s="1">
         <v>36</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C83" s="1">
@@ -3636,7 +3663,7 @@
       <c r="A84" s="1">
         <v>36</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C84" s="1">
@@ -3660,7 +3687,7 @@
       <c r="A85" s="1">
         <v>36</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C85" s="1">
@@ -3686,7 +3713,7 @@
       <c r="A86" s="1">
         <v>36</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C86" s="1">
@@ -3712,7 +3739,7 @@
       <c r="A87" s="1">
         <v>37</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C87" s="1">
@@ -3736,7 +3763,7 @@
       <c r="A88" s="1">
         <v>37</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C88" s="1">
@@ -3760,7 +3787,7 @@
       <c r="A89" s="1">
         <v>38</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C89" s="1">
@@ -3786,7 +3813,7 @@
       <c r="A90" s="1">
         <v>39</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C90" s="1">
@@ -3810,7 +3837,7 @@
       <c r="A91" s="1">
         <v>39</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C91" s="1">
@@ -3834,7 +3861,7 @@
       <c r="A92" s="1">
         <v>39</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C92" s="1">
@@ -3858,7 +3885,7 @@
       <c r="A93" s="1">
         <v>40</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C93" s="1">
@@ -3882,7 +3909,7 @@
       <c r="A94" s="1">
         <v>40</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B94" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C94" s="1">
@@ -3908,7 +3935,7 @@
       <c r="A95" s="1">
         <v>40</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C95" s="1">
@@ -3934,7 +3961,7 @@
       <c r="A96" s="1">
         <v>41</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C96" s="1">
@@ -3958,7 +3985,7 @@
       <c r="A97" s="1">
         <v>41</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C97" s="1">
@@ -3984,7 +4011,7 @@
       <c r="A98" s="1">
         <v>42</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B98" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C98" s="1">
@@ -4008,7 +4035,7 @@
       <c r="A99" s="1">
         <v>42</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B99" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C99" s="1">
@@ -4034,7 +4061,7 @@
       <c r="A100" s="1">
         <v>43</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C100" s="1">
@@ -4058,7 +4085,7 @@
       <c r="A101" s="1">
         <v>43</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B101" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C101" s="1">
@@ -4084,7 +4111,7 @@
       <c r="A102" s="1">
         <v>46</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B102" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C102" s="1">
@@ -4110,7 +4137,7 @@
       <c r="A103" s="1">
         <v>47</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B103" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C103" s="1">
@@ -4134,7 +4161,7 @@
       <c r="A104" s="1">
         <v>47</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B104" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C104" s="1">
@@ -4158,7 +4185,7 @@
       <c r="A105" s="1">
         <v>47</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="B105" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C105" s="1">
@@ -4184,7 +4211,7 @@
       <c r="A106" s="1">
         <v>47</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C106" s="1">
@@ -4210,7 +4237,7 @@
       <c r="A107" s="1">
         <v>49</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B107" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C107" s="1">
@@ -4236,7 +4263,7 @@
       <c r="A108" s="1">
         <v>50</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C108" s="1">
@@ -4262,7 +4289,7 @@
       <c r="A109" s="1">
         <v>51</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C109" s="1">
@@ -4288,7 +4315,7 @@
       <c r="A110" s="1">
         <v>44</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B110" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C110" s="1">
@@ -4314,7 +4341,7 @@
       <c r="A111" s="1">
         <v>52</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C111" s="1">
@@ -4340,7 +4367,7 @@
       <c r="A112" s="1">
         <v>52</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C112" s="1">
@@ -4366,7 +4393,7 @@
       <c r="A113" s="1">
         <v>53</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C113" s="1">
@@ -4392,7 +4419,7 @@
       <c r="A114" s="1">
         <v>54</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B114" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C114" s="1">
@@ -4418,7 +4445,7 @@
       <c r="A115" s="1">
         <v>55</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B115" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C115" s="1">
@@ -4444,7 +4471,7 @@
       <c r="A116" s="1">
         <v>55</v>
       </c>
-      <c r="B116" s="3" t="s">
+      <c r="B116" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C116" s="1">
@@ -4468,7 +4495,7 @@
       <c r="A117" s="1">
         <v>45</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B117" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C117" s="1">
@@ -4494,7 +4521,7 @@
       <c r="A118" s="1">
         <v>45</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C118" s="1">
@@ -4518,7 +4545,7 @@
       <c r="A119" s="1">
         <v>48</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B119" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C119" s="1">
@@ -4544,7 +4571,7 @@
       <c r="A120" s="1">
         <v>48</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C120" s="1">
@@ -4568,7 +4595,7 @@
       <c r="A121" s="1">
         <v>48</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B121" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C121" s="1">
@@ -4594,7 +4621,7 @@
       <c r="A122" s="1">
         <v>48</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B122" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C122" s="1">
@@ -4620,7 +4647,7 @@
       <c r="A123" s="1">
         <v>48</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B123" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C123" s="1">
@@ -4646,7 +4673,7 @@
       <c r="A124" s="1">
         <v>57</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B124" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C124" s="1">
@@ -4670,7 +4697,7 @@
       <c r="A125" s="1">
         <v>57</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B125" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C125" s="1">
@@ -4694,7 +4721,7 @@
       <c r="A126" s="1">
         <v>57</v>
       </c>
-      <c r="B126" s="3" t="s">
+      <c r="B126" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C126" s="1">
@@ -4718,7 +4745,7 @@
       <c r="A127" s="1">
         <v>57</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B127" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C127" s="1">
@@ -4744,7 +4771,7 @@
       <c r="A128" s="1">
         <v>57</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B128" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C128" s="1">
@@ -4770,7 +4797,7 @@
       <c r="A129" s="1">
         <v>57</v>
       </c>
-      <c r="B129" s="3" t="s">
+      <c r="B129" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C129" s="1">
@@ -4796,7 +4823,7 @@
       <c r="A130" s="1">
         <v>57</v>
       </c>
-      <c r="B130" s="3" t="s">
+      <c r="B130" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C130" s="1">
@@ -4822,7 +4849,7 @@
       <c r="A131" s="1">
         <v>58</v>
       </c>
-      <c r="B131" s="3" t="s">
+      <c r="B131" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C131" s="1">
@@ -4846,7 +4873,7 @@
       <c r="A132" s="1">
         <v>59</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="B132" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C132" s="1">
@@ -4872,7 +4899,7 @@
       <c r="A133" s="1">
         <v>59</v>
       </c>
-      <c r="B133" s="3" t="s">
+      <c r="B133" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C133" s="1">
@@ -4898,7 +4925,7 @@
       <c r="A134" s="1">
         <v>60</v>
       </c>
-      <c r="B134" s="3" t="s">
+      <c r="B134" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C134" s="1">
@@ -4924,7 +4951,7 @@
       <c r="A135" s="1">
         <v>60</v>
       </c>
-      <c r="B135" s="3" t="s">
+      <c r="B135" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C135" s="1">
@@ -4950,7 +4977,7 @@
       <c r="A136" s="1">
         <v>60</v>
       </c>
-      <c r="B136" s="3" t="s">
+      <c r="B136" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C136" s="1">
@@ -4976,7 +5003,7 @@
       <c r="A137" s="1">
         <v>61</v>
       </c>
-      <c r="B137" s="3" t="s">
+      <c r="B137" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C137" s="1">
@@ -5000,7 +5027,7 @@
       <c r="A138" s="1">
         <v>61</v>
       </c>
-      <c r="B138" s="3" t="s">
+      <c r="B138" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C138" s="1">
@@ -5024,7 +5051,7 @@
       <c r="A139" s="1">
         <v>61</v>
       </c>
-      <c r="B139" s="3" t="s">
+      <c r="B139" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C139" s="1">
@@ -5048,7 +5075,7 @@
       <c r="A140" s="1">
         <v>62</v>
       </c>
-      <c r="B140" s="3" t="s">
+      <c r="B140" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C140" s="1">
@@ -5074,7 +5101,7 @@
       <c r="A141" s="1">
         <v>62</v>
       </c>
-      <c r="B141" s="3" t="s">
+      <c r="B141" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C141" s="1">
@@ -5100,7 +5127,7 @@
       <c r="A142" s="1">
         <v>63</v>
       </c>
-      <c r="B142" s="3" t="s">
+      <c r="B142" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C142" s="1">
@@ -5117,14 +5144,14 @@
       </c>
       <c r="G142" s="1"/>
       <c r="H142">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>63</v>
       </c>
-      <c r="B143" s="3" t="s">
+      <c r="B143" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C143" s="1">
@@ -5143,14 +5170,14 @@
         <v>126</v>
       </c>
       <c r="H143">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>63</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B144" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C144" s="1">
@@ -5169,14 +5196,14 @@
         <v>126</v>
       </c>
       <c r="H144">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>63</v>
       </c>
-      <c r="B145" s="3" t="s">
+      <c r="B145" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C145" s="1">
@@ -5193,14 +5220,14 @@
       </c>
       <c r="G145" s="1"/>
       <c r="H145">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>63</v>
       </c>
-      <c r="B146" s="3" t="s">
+      <c r="B146" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C146" s="1">
@@ -5217,14 +5244,14 @@
       </c>
       <c r="G146" s="1"/>
       <c r="H146">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>63</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B147" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C147" s="1">
@@ -5241,14 +5268,14 @@
       </c>
       <c r="G147" s="1"/>
       <c r="H147">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>63</v>
       </c>
-      <c r="B148" s="3" t="s">
+      <c r="B148" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C148" s="1">
@@ -5265,14 +5292,14 @@
       </c>
       <c r="G148" s="1"/>
       <c r="H148">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>63</v>
       </c>
-      <c r="B149" s="3" t="s">
+      <c r="B149" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C149" s="1">
@@ -5289,14 +5316,14 @@
       </c>
       <c r="G149" s="1"/>
       <c r="H149">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>63</v>
       </c>
-      <c r="B150" s="3" t="s">
+      <c r="B150" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C150" s="1">
@@ -5315,14 +5342,14 @@
         <v>126</v>
       </c>
       <c r="H150">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>64</v>
       </c>
-      <c r="B151" s="3" t="s">
+      <c r="B151" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C151" s="1">
@@ -5341,14 +5368,14 @@
         <v>126</v>
       </c>
       <c r="H151">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>65</v>
       </c>
-      <c r="B152" s="3" t="s">
+      <c r="B152" s="2" t="s">
         <v>266</v>
       </c>
       <c r="C152" s="1">
@@ -5367,14 +5394,14 @@
         <v>126</v>
       </c>
       <c r="H152">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>65</v>
       </c>
-      <c r="B153" s="3" t="s">
+      <c r="B153" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C153" s="1">
@@ -5391,14 +5418,14 @@
       </c>
       <c r="G153" s="1"/>
       <c r="H153">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>66</v>
       </c>
-      <c r="B154" s="3" t="s">
+      <c r="B154" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C154" s="1">
@@ -5415,14 +5442,14 @@
       </c>
       <c r="G154" s="1"/>
       <c r="H154">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>66</v>
       </c>
-      <c r="B155" s="3" t="s">
+      <c r="B155" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C155" s="1">
@@ -5439,14 +5466,14 @@
       </c>
       <c r="G155" s="1"/>
       <c r="H155">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>67</v>
-      </c>
-      <c r="B156" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>267</v>
       </c>
       <c r="C156" s="1">
@@ -5463,10 +5490,333 @@
       </c>
       <c r="G156" s="1"/>
       <c r="H156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>63</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C157" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>64</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C158" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>64</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C159" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>64</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C160" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>63</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C161" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>63</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C162" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>67</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C163" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>63</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C164" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>64</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C165" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>63</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C166" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>63</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C167" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>63</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C168" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>67</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C169" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>63</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C170" s="1">
+        <v>21000</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H170">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="G1:G2 G4:G5 G150:G152 G143:G144 G127:G130 G132:G136 G121:G123 G119 G117 G105:G115 G101:G102 G94:G95 G97 G99 G85:G86 G89 G69:G83 G55:G61 G44:G47 G32:G42 G27:G30 G23:G25 G9:G11 G15" numberStoredAsText="1"/>
@@ -5477,10 +5827,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2ADEB89-6016-4961-855F-B6B0FA6DB09E}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5488,744 +5838,916 @@
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>195</v>
       </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>196</v>
       </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>197</v>
       </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>198</v>
       </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>199</v>
       </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>200</v>
       </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>201</v>
       </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>202</v>
       </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>203</v>
       </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>204</v>
       </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>3</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>205</v>
       </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>3</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>206</v>
       </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>3</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>207</v>
       </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>3</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>208</v>
       </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>209</v>
       </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>3</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>4</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>4</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>4</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>4</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>5</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>5</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>5</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>5</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>6</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>6</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>6</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>2</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>6</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>6</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>2</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>6</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>6</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>6</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>6</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>2</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>6</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>2</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>7</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>8</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>8</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>8</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>2</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>9</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>10</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>10</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>3</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>10</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>11</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>3</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>11</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>11</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>3</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>12</v>
-      </c>
-      <c r="B46">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1">
         <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>12</v>
-      </c>
-      <c r="B47">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1">
         <v>3</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>12</v>
-      </c>
-      <c r="B48">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>12</v>
+      </c>
+      <c r="B48" s="1">
         <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>13</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>3</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>14</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>3</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>14</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>3</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>14</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>3</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
         <v>14</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>3</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>14</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>3</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>15</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <v>3</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <v>15</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <v>3</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>16</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <v>4</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>9</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <v>5</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>17</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
         <v>5</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>17</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <v>5</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>4</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
         <v>5</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
         <v>18</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="1">
         <v>6</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
         <v>19</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="1">
         <v>6</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="D63" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>19</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="1">
         <v>6</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
+      <c r="D64" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
         <v>19</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="1">
         <v>6</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66">
+      <c r="D65" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
         <v>19</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="1">
         <v>6</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="D66" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
         <v>19</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="1">
         <v>6</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>19</v>
+      </c>
+      <c r="B68" s="1">
+        <v>6</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>255</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to database and courses
added an availability check for courses and added the new courses to the database
</commit_message>
<xml_diff>
--- a/Database/Data/database.xlsx
+++ b/Database/Data/database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\PycharmProjects\PirieBot\Database\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A64B13A-35B1-4E2A-AEDA-6EDD07233520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D96222-B5EE-4583-8F67-D526F1D5C650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,6 +114,7 @@
     <author>tc={B3D325A7-DD65-451D-975F-32B8A78690EE}</author>
     <author>tc={40FE144C-D2CB-4BCE-B7E5-E087CBF13956}</author>
     <author>tc={BA83BE48-2326-4572-B975-ED8DFC153836}</author>
+    <author>tc={386A11B9-684C-4927-846B-0B394B2BFDC5}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{948D2A91-26FC-4A9E-A133-BFA6225ED9FD}">
@@ -154,6 +155,14 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     description</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="5" shapeId="0" xr:uid="{386A11B9-684C-4927-846B-0B394B2BFDC5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    availability</t>
       </text>
     </comment>
   </commentList>
@@ -215,7 +224,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="291">
   <si>
     <t>S: 10:30 am - 11:30 am</t>
   </si>
@@ -1046,13 +1055,55 @@
   </si>
   <si>
     <t>Este curso es reconocido por el Servicio Civil por lo que es importante que no faltes a las clases o justifiques y repongas las lecciones a las que te ausentes.</t>
+  </si>
+  <si>
+    <t>Busca fomentar hábitos alimentarios para una alimentación sostenible, dichos hábitos deben de ser saludables para promover una adecuada escogencia de alimentos y por ende mejorar la conducta alimentaria. Se incluyen temas de alimentación en diferentes grupos de edad, lectura de etiquetas, mitos alimentarios, alimentación para diferentes enfermedades, manipulación de alimentos, entre otros.</t>
+  </si>
+  <si>
+    <t>Este curso se da cada tres meses por lo que es importante que no faltes a clases o justifiques las ausencias para programar reposiciones.</t>
+  </si>
+  <si>
+    <t>Ana Guillen</t>
+  </si>
+  <si>
+    <t>Bordado Principiantes</t>
+  </si>
+  <si>
+    <t>Quilting Principiantes</t>
+  </si>
+  <si>
+    <t>Se aprende a armar, cortar, coser, armar y acolchar utilizando diferentes técnicas, a usar cuchilla y reglas. Los trabajos son realizados con telas de algodón, se pueden realizar colchas, caminos de mesa, entre otros. Según se avance en los niveles, los bloques de trabajo aumentan la dificultad y aumentan la variedad de técnicas, tales como estilo vitral, crazy quilt y otras.</t>
+  </si>
+  <si>
+    <t>Los mismos docentes prefieren hablar al respecto en la primera clase (en el caso de los cursos que requieren del uso de herramientas y materiales), esto con el fin de que puedan ser asesorados y asesoradas correctamente por la o el mismo docente y que cada estudiante haga una mejor inversión de su dinero, tanto a nivel de calidad como de economía.</t>
+  </si>
+  <si>
+    <t>L: 4:00 pm - 5:50 pm</t>
+  </si>
+  <si>
+    <t>L: 2:00 pm - 3:50 pm</t>
+  </si>
+  <si>
+    <t>M: 2:00 pm - 3:50 pm</t>
+  </si>
+  <si>
+    <t>M: 5:00 pm - 6:50 pm</t>
+  </si>
+  <si>
+    <t>J: 2:00 pm - 3:50 pm</t>
+  </si>
+  <si>
+    <t>J: 5:00 pm - 6:50 pm</t>
+  </si>
+  <si>
+    <t>V: 5:00 pm - 6:50 pm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1072,6 +1123,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1493,6 +1550,9 @@
   <threadedComment ref="E1" dT="2023-03-24T20:53:49.73" personId="{6DF7EF9A-B3A0-4845-92B8-B81FE36C707F}" id="{BA83BE48-2326-4572-B975-ED8DFC153836}">
     <text>description</text>
   </threadedComment>
+  <threadedComment ref="F1" dT="2023-04-17T22:13:40.35" personId="{6DF7EF9A-B3A0-4845-92B8-B81FE36C707F}" id="{386A11B9-684C-4927-846B-0B394B2BFDC5}">
+    <text>availability</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1520,10 +1580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H170"/>
+  <dimension ref="A1:H178"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I156" sqref="I156"/>
+    <sheetView topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="H151" sqref="H151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,7 +1620,7 @@
         <v>3</v>
       </c>
       <c r="H1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1586,7 +1646,7 @@
         <v>3</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1610,7 +1670,7 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1636,7 +1696,7 @@
         <v>3</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1662,7 +1722,7 @@
         <v>3</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1688,7 +1748,7 @@
         <v>256</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1714,7 +1774,7 @@
         <v>256</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1740,7 +1800,7 @@
         <v>256</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1766,7 +1826,7 @@
         <v>19</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1792,7 +1852,7 @@
         <v>19</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1818,7 +1878,7 @@
         <v>19</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1844,7 +1904,7 @@
         <v>256</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1870,7 +1930,7 @@
         <v>256</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1896,7 +1956,7 @@
         <v>256</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1922,7 +1982,7 @@
         <v>19</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1948,7 +2008,7 @@
         <v>256</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1974,7 +2034,7 @@
         <v>256</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2000,7 +2060,7 @@
         <v>256</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2026,7 +2086,7 @@
         <v>256</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2052,7 +2112,7 @@
         <v>256</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2078,7 +2138,7 @@
         <v>256</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2104,7 +2164,7 @@
         <v>256</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2130,7 +2190,7 @@
         <v>19</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2156,7 +2216,7 @@
         <v>19</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2182,7 +2242,7 @@
         <v>19</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2206,7 +2266,7 @@
       </c>
       <c r="G26" s="1"/>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2232,7 +2292,7 @@
         <v>43</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2258,7 +2318,7 @@
         <v>19</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2284,7 +2344,7 @@
         <v>43</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2310,7 +2370,7 @@
         <v>19</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2334,7 +2394,7 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2360,7 +2420,7 @@
         <v>19</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2386,7 +2446,7 @@
         <v>19</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2412,7 +2472,7 @@
         <v>19</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2438,7 +2498,7 @@
         <v>43</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2464,7 +2524,7 @@
         <v>54</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2490,7 +2550,7 @@
         <v>54</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2516,7 +2576,7 @@
         <v>54</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2542,7 +2602,7 @@
         <v>54</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2568,7 +2628,7 @@
         <v>54</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2594,7 +2654,7 @@
         <v>54</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2620,7 +2680,7 @@
         <v>54</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2644,7 +2704,7 @@
       </c>
       <c r="G43" s="1"/>
       <c r="H43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2670,7 +2730,7 @@
         <v>54</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2696,7 +2756,7 @@
         <v>54</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2722,7 +2782,7 @@
         <v>54</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -2748,7 +2808,7 @@
         <v>54</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -2772,7 +2832,7 @@
       </c>
       <c r="G48" s="1"/>
       <c r="H48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2796,7 +2856,7 @@
       </c>
       <c r="G49" s="1"/>
       <c r="H49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2820,7 +2880,7 @@
       </c>
       <c r="G50" s="1"/>
       <c r="H50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2844,7 +2904,7 @@
       </c>
       <c r="G51" s="1"/>
       <c r="H51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2868,7 +2928,7 @@
       </c>
       <c r="G52" s="1"/>
       <c r="H52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2892,7 +2952,7 @@
       </c>
       <c r="G53" s="1"/>
       <c r="H53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2916,7 +2976,7 @@
       </c>
       <c r="G54" s="1"/>
       <c r="H54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2942,7 +3002,7 @@
         <v>75</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2968,7 +3028,7 @@
         <v>75</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2994,7 +3054,7 @@
         <v>75</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3020,7 +3080,7 @@
         <v>75</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -3046,7 +3106,7 @@
         <v>75</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -3072,7 +3132,7 @@
         <v>75</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -3098,7 +3158,7 @@
         <v>75</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3122,7 +3182,7 @@
       </c>
       <c r="G62" s="1"/>
       <c r="H62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -3146,7 +3206,7 @@
       </c>
       <c r="G63" s="1"/>
       <c r="H63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3170,7 +3230,7 @@
       </c>
       <c r="G64" s="1"/>
       <c r="H64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3194,7 +3254,7 @@
       </c>
       <c r="G65" s="1"/>
       <c r="H65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -3218,7 +3278,7 @@
       </c>
       <c r="G66" s="1"/>
       <c r="H66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3242,7 +3302,7 @@
       </c>
       <c r="G67" s="1"/>
       <c r="H67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -3266,7 +3326,7 @@
       </c>
       <c r="G68" s="1"/>
       <c r="H68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -3292,7 +3352,7 @@
         <v>75</v>
       </c>
       <c r="H69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -3318,7 +3378,7 @@
         <v>75</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -3344,7 +3404,7 @@
         <v>75</v>
       </c>
       <c r="H71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -3370,7 +3430,7 @@
         <v>75</v>
       </c>
       <c r="H72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -3396,7 +3456,7 @@
         <v>75</v>
       </c>
       <c r="H73">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -3422,7 +3482,7 @@
         <v>75</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3448,7 +3508,7 @@
         <v>75</v>
       </c>
       <c r="H75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3474,7 +3534,7 @@
         <v>75</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3500,7 +3560,7 @@
         <v>75</v>
       </c>
       <c r="H77">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3526,7 +3586,7 @@
         <v>75</v>
       </c>
       <c r="H78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3552,7 +3612,7 @@
         <v>75</v>
       </c>
       <c r="H79">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3578,7 +3638,7 @@
         <v>75</v>
       </c>
       <c r="H80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3604,7 +3664,7 @@
         <v>75</v>
       </c>
       <c r="H81">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -3630,7 +3690,7 @@
         <v>75</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3656,7 +3716,7 @@
         <v>103</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -3680,7 +3740,7 @@
       </c>
       <c r="G84" s="1"/>
       <c r="H84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3706,7 +3766,7 @@
         <v>103</v>
       </c>
       <c r="H85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -3732,7 +3792,7 @@
         <v>103</v>
       </c>
       <c r="H86">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3756,7 +3816,7 @@
       </c>
       <c r="G87" s="1"/>
       <c r="H87">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3780,7 +3840,7 @@
       </c>
       <c r="G88" s="1"/>
       <c r="H88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3806,7 +3866,7 @@
         <v>103</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3830,7 +3890,7 @@
       </c>
       <c r="G90" s="1"/>
       <c r="H90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3854,7 +3914,7 @@
       </c>
       <c r="G91" s="1"/>
       <c r="H91">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -3878,7 +3938,7 @@
       </c>
       <c r="G92" s="1"/>
       <c r="H92">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -3902,7 +3962,7 @@
       </c>
       <c r="G93" s="1"/>
       <c r="H93">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3928,7 +3988,7 @@
         <v>111</v>
       </c>
       <c r="H94">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -3954,7 +4014,7 @@
         <v>111</v>
       </c>
       <c r="H95">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3978,7 +4038,7 @@
       </c>
       <c r="G96" s="1"/>
       <c r="H96">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -4004,7 +4064,7 @@
         <v>111</v>
       </c>
       <c r="H97">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -4028,7 +4088,7 @@
       </c>
       <c r="G98" s="1"/>
       <c r="H98">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -4054,7 +4114,7 @@
         <v>111</v>
       </c>
       <c r="H99">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -4078,7 +4138,7 @@
       </c>
       <c r="G100" s="1"/>
       <c r="H100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4104,7 +4164,7 @@
         <v>119</v>
       </c>
       <c r="H101">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -4130,7 +4190,7 @@
         <v>121</v>
       </c>
       <c r="H102">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -4154,7 +4214,7 @@
       </c>
       <c r="G103" s="1"/>
       <c r="H103">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -4178,7 +4238,7 @@
       </c>
       <c r="G104" s="1"/>
       <c r="H104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -4204,7 +4264,7 @@
         <v>121</v>
       </c>
       <c r="H105">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -4230,7 +4290,7 @@
         <v>121</v>
       </c>
       <c r="H106">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -4256,7 +4316,7 @@
         <v>126</v>
       </c>
       <c r="H107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -4282,7 +4342,7 @@
         <v>129</v>
       </c>
       <c r="H108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -4308,7 +4368,7 @@
         <v>129</v>
       </c>
       <c r="H109">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -4334,7 +4394,7 @@
         <v>119</v>
       </c>
       <c r="H110">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -4360,7 +4420,7 @@
         <v>129</v>
       </c>
       <c r="H111">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -4386,7 +4446,7 @@
         <v>129</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -4412,7 +4472,7 @@
         <v>129</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -4438,7 +4498,7 @@
         <v>129</v>
       </c>
       <c r="H114">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -4464,7 +4524,7 @@
         <v>119</v>
       </c>
       <c r="H115">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -4488,7 +4548,7 @@
       </c>
       <c r="G116" s="1"/>
       <c r="H116">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -4514,7 +4574,7 @@
         <v>111</v>
       </c>
       <c r="H117">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -4538,7 +4598,7 @@
       </c>
       <c r="G118" s="1"/>
       <c r="H118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -4564,7 +4624,7 @@
         <v>111</v>
       </c>
       <c r="H119">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -4588,7 +4648,7 @@
       </c>
       <c r="G120" s="1"/>
       <c r="H120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -4614,7 +4674,7 @@
         <v>111</v>
       </c>
       <c r="H121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -4640,7 +4700,7 @@
         <v>111</v>
       </c>
       <c r="H122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -4666,7 +4726,7 @@
         <v>111</v>
       </c>
       <c r="H123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -4690,7 +4750,7 @@
       </c>
       <c r="G124" s="1"/>
       <c r="H124">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -4714,7 +4774,7 @@
       </c>
       <c r="G125" s="1"/>
       <c r="H125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -4738,7 +4798,7 @@
       </c>
       <c r="G126" s="1"/>
       <c r="H126">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -4764,7 +4824,7 @@
         <v>119</v>
       </c>
       <c r="H127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -4790,7 +4850,7 @@
         <v>119</v>
       </c>
       <c r="H128">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -4816,7 +4876,7 @@
         <v>119</v>
       </c>
       <c r="H129">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -4842,7 +4902,7 @@
         <v>119</v>
       </c>
       <c r="H130">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -4866,7 +4926,7 @@
       </c>
       <c r="G131" s="1"/>
       <c r="H131">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -4892,7 +4952,7 @@
         <v>150</v>
       </c>
       <c r="H132">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -4918,7 +4978,7 @@
         <v>150</v>
       </c>
       <c r="H133">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -4944,7 +5004,7 @@
         <v>150</v>
       </c>
       <c r="H134">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -4970,7 +5030,7 @@
         <v>150</v>
       </c>
       <c r="H135">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -4996,7 +5056,7 @@
         <v>150</v>
       </c>
       <c r="H136">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -5020,7 +5080,7 @@
       </c>
       <c r="G137" s="1"/>
       <c r="H137">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -5044,7 +5104,7 @@
       </c>
       <c r="G138" s="1"/>
       <c r="H138">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -5068,7 +5128,7 @@
       </c>
       <c r="G139" s="1"/>
       <c r="H139">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -5094,7 +5154,7 @@
         <v>257</v>
       </c>
       <c r="H140">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -5120,7 +5180,7 @@
         <v>257</v>
       </c>
       <c r="H141">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -5812,6 +5872,190 @@
         <v>148</v>
       </c>
       <c r="H170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>58</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C171" s="1">
+        <v>18000</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>69</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C172" s="1">
+        <v>19350</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>70</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C173" s="1">
+        <v>19350</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>70</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C174" s="1">
+        <v>19350</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>70</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C175" s="1">
+        <v>19350</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>70</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C176" s="1">
+        <v>19350</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>70</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C177" s="1">
+        <v>19350</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>70</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C178" s="1">
+        <v>19350</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H178">
         <v>1</v>
       </c>
     </row>
@@ -5827,10 +6071,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2ADEB89-6016-4961-855F-B6B0FA6DB09E}">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5838,11 +6082,11 @@
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" customWidth="1"/>
     <col min="5" max="5" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -5854,8 +6098,11 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -5867,8 +6114,11 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5880,8 +6130,11 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -5893,8 +6146,11 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -5906,8 +6162,11 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -5919,8 +6178,11 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -5932,8 +6194,11 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -5945,8 +6210,11 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -5958,8 +6226,11 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -5971,8 +6242,11 @@
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -5984,8 +6258,11 @@
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -5997,8 +6274,11 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -6010,8 +6290,11 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -6023,8 +6306,11 @@
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -6036,8 +6322,11 @@
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -6049,8 +6338,11 @@
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>4</v>
       </c>
@@ -6062,8 +6354,11 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -6075,8 +6370,11 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>4</v>
       </c>
@@ -6088,8 +6386,11 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>4</v>
       </c>
@@ -6101,8 +6402,11 @@
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>5</v>
       </c>
@@ -6114,8 +6418,11 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>5</v>
       </c>
@@ -6127,8 +6434,11 @@
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>5</v>
       </c>
@@ -6140,8 +6450,11 @@
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>5</v>
       </c>
@@ -6153,8 +6466,11 @@
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>6</v>
       </c>
@@ -6166,8 +6482,11 @@
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>6</v>
       </c>
@@ -6179,8 +6498,11 @@
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>6</v>
       </c>
@@ -6192,8 +6514,11 @@
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>6</v>
       </c>
@@ -6205,8 +6530,11 @@
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>6</v>
       </c>
@@ -6218,8 +6546,11 @@
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>6</v>
       </c>
@@ -6231,8 +6562,11 @@
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>6</v>
       </c>
@@ -6244,8 +6578,11 @@
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>6</v>
       </c>
@@ -6257,8 +6594,11 @@
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>6</v>
       </c>
@@ -6270,8 +6610,11 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>6</v>
       </c>
@@ -6283,8 +6626,11 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>7</v>
       </c>
@@ -6296,8 +6642,11 @@
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>8</v>
       </c>
@@ -6309,8 +6658,11 @@
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>8</v>
       </c>
@@ -6322,8 +6674,11 @@
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>8</v>
       </c>
@@ -6335,8 +6690,11 @@
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>9</v>
       </c>
@@ -6348,8 +6706,11 @@
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>10</v>
       </c>
@@ -6361,8 +6722,11 @@
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>10</v>
       </c>
@@ -6374,8 +6738,11 @@
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>10</v>
       </c>
@@ -6387,8 +6754,11 @@
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>11</v>
       </c>
@@ -6400,8 +6770,11 @@
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>11</v>
       </c>
@@ -6413,8 +6786,11 @@
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>11</v>
       </c>
@@ -6426,8 +6802,11 @@
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>12</v>
       </c>
@@ -6439,8 +6818,11 @@
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>12</v>
       </c>
@@ -6452,8 +6834,11 @@
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>12</v>
       </c>
@@ -6465,8 +6850,11 @@
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>13</v>
       </c>
@@ -6478,8 +6866,11 @@
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>14</v>
       </c>
@@ -6491,8 +6882,11 @@
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>14</v>
       </c>
@@ -6504,8 +6898,11 @@
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>14</v>
       </c>
@@ -6517,8 +6914,11 @@
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>14</v>
       </c>
@@ -6530,8 +6930,11 @@
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>14</v>
       </c>
@@ -6543,8 +6946,11 @@
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>15</v>
       </c>
@@ -6556,8 +6962,11 @@
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>15</v>
       </c>
@@ -6569,8 +6978,11 @@
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>16</v>
       </c>
@@ -6582,8 +6994,11 @@
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>9</v>
       </c>
@@ -6593,10 +7008,17 @@
       <c r="C58" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D58" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>17</v>
       </c>
@@ -6608,8 +7030,11 @@
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>17</v>
       </c>
@@ -6621,8 +7046,11 @@
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>4</v>
       </c>
@@ -6634,8 +7062,11 @@
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>18</v>
       </c>
@@ -6647,8 +7078,11 @@
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>19</v>
       </c>
@@ -6664,8 +7098,11 @@
       <c r="E63" s="3" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>19</v>
       </c>
@@ -6681,8 +7118,11 @@
       <c r="E64" s="3" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>19</v>
       </c>
@@ -6698,8 +7138,11 @@
       <c r="E65" s="3" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>19</v>
       </c>
@@ -6715,8 +7158,11 @@
       <c r="E66" s="3" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>19</v>
       </c>
@@ -6732,8 +7178,11 @@
       <c r="E67" s="3" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>19</v>
       </c>
@@ -6748,6 +7197,49 @@
       </c>
       <c r="E68" s="3" t="s">
         <v>275</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>20</v>
+      </c>
+      <c r="B69" s="1">
+        <v>4</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D69">
+        <v>404</v>
+      </c>
+      <c r="E69">
+        <v>404</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>20</v>
+      </c>
+      <c r="B70" s="1">
+        <v>4</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6759,10 +7251,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B558BCCB-B295-4555-AF6A-EC02D1057D3C}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6945,10 +7437,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>178</v>
+        <v>279</v>
       </c>
       <c r="C20" s="1"/>
     </row>
@@ -6957,9 +7449,18 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>